<commit_message>
rjb3.rb for image read/store
</commit_message>
<xml_diff>
--- a/image_import_ralph.xlsx
+++ b/image_import_ralph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20475" windowHeight="8085"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -360,15 +360,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3333750</xdr:colOff>
+      <xdr:colOff>3733800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>2133600</xdr:rowOff>
+      <xdr:rowOff>2178255</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -392,8 +392,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4619625" y="323850"/>
-          <a:ext cx="3238500" cy="2152650"/>
+          <a:off x="5124450" y="266700"/>
+          <a:ext cx="3133725" cy="2083005"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -428,15 +428,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4038600</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>3781425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>3571875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -460,8 +460,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4581525" y="2705100"/>
-          <a:ext cx="3981450" cy="2543175"/>
+          <a:off x="4848225" y="2571750"/>
+          <a:ext cx="3457575" cy="3457575"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -496,15 +496,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>2466975</xdr:rowOff>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3886200</xdr:colOff>
+      <xdr:colOff>3648075</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2933700</xdr:rowOff>
+      <xdr:rowOff>3310979</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -528,8 +528,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4752975" y="5086350"/>
-          <a:ext cx="3657600" cy="2933700"/>
+          <a:off x="5572125" y="6562725"/>
+          <a:ext cx="2600325" cy="3101429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -564,15 +564,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>371475</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>600075</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4162425</xdr:colOff>
+      <xdr:colOff>4486275</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>3381375</xdr:rowOff>
+      <xdr:rowOff>3790950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -596,7 +596,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4572000" y="8782050"/>
+          <a:off x="4895850" y="10458450"/>
           <a:ext cx="4114800" cy="3190875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -632,15 +632,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>438150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4114800</xdr:colOff>
+      <xdr:colOff>4572000</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>2524125</xdr:rowOff>
+      <xdr:rowOff>2933700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -664,7 +664,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4543425" y="12620625"/>
+          <a:off x="5000625" y="14297025"/>
           <a:ext cx="4095750" cy="2495550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -700,15 +700,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>4010025</xdr:rowOff>
+      <xdr:colOff>762001</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>551709</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4210050</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2762250</xdr:rowOff>
+      <xdr:rowOff>3589808</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -732,8 +732,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4524375" y="16602075"/>
-          <a:ext cx="4657725" cy="2762250"/>
+          <a:off x="5286376" y="17953884"/>
+          <a:ext cx="3448049" cy="3038099"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -768,15 +768,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>390525</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>352425</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4143375</xdr:colOff>
+      <xdr:colOff>4533900</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2238375</xdr:rowOff>
+      <xdr:rowOff>2590800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -800,7 +800,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4524375" y="19431000"/>
+          <a:off x="4914900" y="22345650"/>
           <a:ext cx="4143375" cy="2238375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -836,15 +836,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>3829050</xdr:rowOff>
+      <xdr:colOff>361949</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>120014</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4286250</xdr:colOff>
+      <xdr:colOff>4352924</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>2495550</xdr:rowOff>
+      <xdr:rowOff>2514599</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -868,8 +868,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4619625" y="23260050"/>
-          <a:ext cx="4191000" cy="2514600"/>
+          <a:off x="4886324" y="25961339"/>
+          <a:ext cx="3990975" cy="2394585"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -903,16 +903,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4524375</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>2590800</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>4095750</xdr:colOff>
+      <xdr:colOff>4238625</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>2895600</xdr:rowOff>
+      <xdr:rowOff>3009900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -936,7 +936,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4524375" y="25869900"/>
+          <a:off x="4667250" y="28546425"/>
           <a:ext cx="4095750" cy="2895600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -971,16 +971,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4524375</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>3238500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3524250</xdr:colOff>
+      <xdr:colOff>3743325</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>2647950</xdr:rowOff>
+      <xdr:rowOff>2924175</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1004,7 +1004,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4524375" y="29108400"/>
+          <a:off x="4743450" y="31946850"/>
           <a:ext cx="3524250" cy="2647950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1040,15 +1040,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>247650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3819525</xdr:colOff>
+      <xdr:colOff>3867150</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>2695575</xdr:rowOff>
+      <xdr:rowOff>2895600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1072,7 +1072,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4876800" y="32394525"/>
+          <a:off x="4924425" y="35156775"/>
           <a:ext cx="3467100" cy="2647950"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1107,16 +1107,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4524375</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>3238500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3162300</xdr:colOff>
+      <xdr:colOff>3371850</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>2686050</xdr:rowOff>
+      <xdr:rowOff>2886075</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1140,7 +1140,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4524375" y="35585400"/>
+          <a:off x="4733925" y="35613975"/>
           <a:ext cx="3162300" cy="2686050"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1175,16 +1175,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4524375</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>3238500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>3457575</xdr:colOff>
+      <xdr:colOff>3667125</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>2800350</xdr:rowOff>
+      <xdr:rowOff>3038475</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1208,7 +1208,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4524375" y="38823900"/>
+          <a:off x="4733925" y="38890575"/>
           <a:ext cx="3457575" cy="2800350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1244,15 +1244,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2085975</xdr:colOff>
+      <xdr:colOff>2428875</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>3152775</xdr:rowOff>
+      <xdr:rowOff>3619500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1276,8 +1276,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4524375" y="42062400"/>
-          <a:ext cx="2085975" cy="3152775"/>
+          <a:off x="4867275" y="44729400"/>
+          <a:ext cx="2085975" cy="3514725"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1601,14 +1601,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="59.375" customWidth="1"/>
-    <col min="2" max="2" width="57.75" customWidth="1"/>
+    <col min="2" max="2" width="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1625,7 +1625,7 @@
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" ht="194.1" customHeight="1">
+    <row r="3" spans="1:2" ht="306.75" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1643,12 +1643,12 @@
       </c>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" ht="315.95" customHeight="1">
+    <row r="6" spans="1:2" ht="279" customHeight="1">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="222.95" customHeight="1">
+    <row r="7" spans="1:2" ht="361.5" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="255" customHeight="1">
+    <row r="15" spans="1:2" ht="301.5" customHeight="1">
       <c r="A15" t="s">
         <v>14</v>
       </c>

</xml_diff>